<commit_message>
Updated sample charts. Works fine on Office for Mac OS but Excel on Windows complains about the drawings but will accept them. Probably need to add validation. The relevant XML files are identical in XML terms.
--HG--
branch : 1.8
</commit_message>
<xml_diff>
--- a/openpyxl/sample/files/charts.xlsx
+++ b/openpyxl/sample/files/charts.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <s:bookViews>
     <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet name="Numbers" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Negative" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Letters" sheetId="3" r:id="rId3"/>
-    <s:sheet name="Dates" sheetId="4" r:id="rId4"/>
-    <s:sheet name="Pie" sheetId="5" r:id="rId5"/>
-    <s:sheet name="Line" sheetId="6" r:id="rId6"/>
-    <s:sheet name="Scatter" sheetId="7" r:id="rId7"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Numbers" sheetId="1" r:id="rId1"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Negative" sheetId="2" r:id="rId2"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Letters" sheetId="3" r:id="rId3"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dates" sheetId="4" r:id="rId4"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pie" sheetId="5" r:id="rId5"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Line" sheetId="6" r:id="rId6"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scatter" sheetId="7" r:id="rId7"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -26,28 +26,28 @@
     <t>A</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
-    <t>B</t>
+    <t>D</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>D</t>
+    <t>F</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
-    <t>F</t>
+    <t>H</t>
   </si>
   <si>
     <t>I</t>
-  </si>
-  <si>
-    <t>H</t>
   </si>
   <si>
     <t>J</t>
@@ -1066,20 +1066,20 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Graphique 0"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
@@ -1091,20 +1091,20 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Graphique 0"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
@@ -1116,20 +1116,20 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Graphique 0"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
@@ -1141,20 +1141,20 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Graphique 0"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
@@ -1166,20 +1166,20 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Graphique 0"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
@@ -1191,20 +1191,20 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Graphique 0"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
@@ -1216,20 +1216,20 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Graphique 0"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
@@ -1245,10 +1245,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1404,7 +1404,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1413,13 +1413,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1429,7 +1429,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1438,7 +1438,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1447,7 +1447,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1457,12 +1457,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1493,7 +1493,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1512,7 +1512,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1536,7 +1536,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" collapsed="0" width="9.10" min="1"/>
+    <col min="1" max="1" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1607,7 +1607,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" collapsed="0" width="9.10" min="1"/>
+    <col min="1" max="1" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1678,9 +1678,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" collapsed="0" width="9.10" min="1"/>
-    <col max="3" collapsed="0" width="9.10" min="3"/>
-    <col max="2" collapsed="0" width="9.10" min="2"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1696,7 +1696,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
         <v>3</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
         <v>5</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
         <v>7</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
         <v>8</v>
@@ -1811,8 +1811,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" collapsed="0" width="9.10" min="1"/>
-    <col max="2" collapsed="0" width="9.10" min="2"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1905,7 +1905,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" collapsed="0" width="9.10" min="1"/>
+    <col min="1" max="1" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1946,7 +1946,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" collapsed="0" width="9.10" min="1"/>
+    <col min="1" max="1" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1987,8 +1987,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col max="1" collapsed="0" width="9.10" min="1"/>
-    <col max="2" collapsed="0" width="9.10" min="2"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
Completely forgot to test
--HG--
branch : 1.8
extra : rebase_source : d3226af03b082217add182d1bded7b6eff6e5487
</commit_message>
<xml_diff>
--- a/openpyxl/sample/files/charts.xlsx
+++ b/openpyxl/sample/files/charts.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <s:bookViews>
     <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Numbers" sheetId="1" r:id="rId1"/>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Negative" sheetId="2" r:id="rId2"/>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Letters" sheetId="3" r:id="rId3"/>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dates" sheetId="4" r:id="rId4"/>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pie" sheetId="5" r:id="rId5"/>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Line" sheetId="6" r:id="rId6"/>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scatter" sheetId="7" r:id="rId7"/>
+    <s:sheet name="Numbers" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Negative" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Letters" sheetId="3" r:id="rId3"/>
+    <s:sheet name="Dates" sheetId="4" r:id="rId4"/>
+    <s:sheet name="Pie" sheetId="5" r:id="rId5"/>
+    <s:sheet name="Line" sheetId="6" r:id="rId6"/>
+    <s:sheet name="Scatter" sheetId="7" r:id="rId7"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -1066,7 +1066,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1076,12 +1076,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
-        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1091,7 +1091,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1101,12 +1101,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
-        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1116,7 +1116,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1126,12 +1126,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
-        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1141,7 +1141,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1151,12 +1151,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
-        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1166,7 +1166,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1176,12 +1176,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
-        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1191,7 +1191,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1201,12 +1201,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
-        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1216,7 +1216,7 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1226,12 +1226,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
-        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1245,10 +1245,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1404,7 +1404,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1413,13 +1413,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1429,7 +1429,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1438,7 +1438,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1447,7 +1447,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1457,12 +1457,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1493,7 +1493,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1512,7 +1512,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1524,68 +1524,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
+    <col min="1" width="9.10" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="n">
+    <row spans="1:1" r="1">
+      <c t="n" r="A1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="n">
+    <row spans="1:1" r="2">
+      <c t="n" r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="n">
+    <row spans="1:1" r="3">
+      <c t="n" r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="n">
+    <row spans="1:1" r="4">
+      <c t="n" r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="n">
+    <row spans="1:1" r="5">
+      <c t="n" r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="n">
+    <row spans="1:1" r="6">
+      <c t="n" r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="n">
+    <row spans="1:1" r="7">
+      <c t="n" r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="n">
+    <row spans="1:1" r="8">
+      <c t="n" r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="n">
+    <row spans="1:1" r="9">
+      <c t="n" r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="n">
+    <row spans="1:1" r="10">
+      <c t="n" r="A10">
         <v>9</v>
       </c>
     </row>
@@ -1595,68 +1595,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
+    <col min="1" width="9.10" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="n">
+    <row spans="1:1" r="1">
+      <c t="n" r="A1">
         <v>-5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="n">
+    <row spans="1:1" r="2">
+      <c t="n" r="A2">
         <v>-4</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="n">
+    <row spans="1:1" r="3">
+      <c t="n" r="A3">
         <v>-3</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="n">
+    <row spans="1:1" r="4">
+      <c t="n" r="A4">
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="n">
+    <row spans="1:1" r="5">
+      <c t="n" r="A5">
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="n">
+    <row spans="1:1" r="6">
+      <c t="n" r="A6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="n">
+    <row spans="1:1" r="7">
+      <c t="n" r="A7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="n">
+    <row spans="1:1" r="8">
+      <c t="n" r="A8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="n">
+    <row spans="1:1" r="9">
+      <c t="n" r="A9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="n">
+    <row spans="1:1" r="10">
+      <c t="n" r="A10">
         <v>4</v>
       </c>
     </row>
@@ -1666,130 +1666,130 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
-    <col min="3" max="3" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
+    <col min="1" width="9.10" max="1"/>
+    <col min="3" width="9.10" max="3"/>
+    <col min="2" width="9.10" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row spans="1:3" r="1">
+      <c t="s" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>0</v>
       </c>
-      <c r="C1" t="n">
+      <c t="n" r="C1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row spans="1:3" r="2">
+      <c t="s" r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row spans="1:3" r="3">
+      <c t="s" r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row spans="1:3" r="4">
+      <c t="s" r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c t="n" r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="n">
+      <c t="n" r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row spans="1:3" r="5">
+      <c t="s" r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c t="n" r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="n">
+      <c t="n" r="C5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row spans="1:3" r="6">
+      <c t="s" r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
+      <c t="n" r="B6">
         <v>5</v>
       </c>
-      <c r="C6" t="n">
+      <c t="n" r="C6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row spans="1:3" r="7">
+      <c t="s" r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c t="n" r="B7">
         <v>6</v>
       </c>
-      <c r="C7" t="n">
+      <c t="n" r="C7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row spans="1:3" r="8">
+      <c t="s" r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c t="n" r="B8">
         <v>7</v>
       </c>
-      <c r="C8" t="n">
+      <c t="n" r="C8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row spans="1:3" r="9">
+      <c t="s" r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
+      <c t="n" r="B9">
         <v>8</v>
       </c>
-      <c r="C9" t="n">
+      <c t="n" r="C9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row spans="1:3" r="10">
+      <c t="s" r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
+      <c t="n" r="B10">
         <v>9</v>
       </c>
-      <c r="C10" t="n">
+      <c t="n" r="C10">
         <v>9</v>
       </c>
     </row>
@@ -1799,91 +1799,91 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
+    <col min="1" width="9.10" max="1"/>
+    <col min="2" width="9.10" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c s="1" r="A1" t="n">
+    <row spans="1:2" r="1">
+      <c t="n" r="A1" s="1">
         <v>41275.0</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c s="1" r="A2" t="n">
+    <row spans="1:2" r="2">
+      <c t="n" r="A2" s="1">
         <v>41306.0</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c s="1" r="A3" t="n">
+    <row spans="1:2" r="3">
+      <c t="n" r="A3" s="1">
         <v>41334.0</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c s="1" r="A4" t="n">
+    <row spans="1:2" r="4">
+      <c t="n" r="A4" s="1">
         <v>41365.0</v>
       </c>
-      <c r="B4" t="n">
+      <c t="n" r="B4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c s="1" r="A5" t="n">
+    <row spans="1:2" r="5">
+      <c t="n" r="A5" s="1">
         <v>41395.0</v>
       </c>
-      <c r="B5" t="n">
+      <c t="n" r="B5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c s="1" r="A6" t="n">
+    <row spans="1:2" r="6">
+      <c t="n" r="A6" s="1">
         <v>41426.0</v>
       </c>
-      <c r="B6" t="n">
+      <c t="n" r="B6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c s="1" r="A7" t="n">
+    <row spans="1:2" r="7">
+      <c t="n" r="A7" s="1">
         <v>41456.0</v>
       </c>
-      <c r="B7" t="n">
+      <c t="n" r="B7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c s="1" r="A8" t="n">
+    <row spans="1:2" r="8">
+      <c t="n" r="A8" s="1">
         <v>41487.0</v>
       </c>
-      <c r="B8" t="n">
+      <c t="n" r="B8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c s="1" r="A9" t="n">
+    <row spans="1:2" r="9">
+      <c t="n" r="A9" s="1">
         <v>41518.0</v>
       </c>
-      <c r="B9" t="n">
+      <c t="n" r="B9">
         <v>9</v>
       </c>
     </row>
@@ -1893,38 +1893,38 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
+    <col min="1" width="9.10" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="n">
+    <row spans="1:1" r="1">
+      <c t="n" r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="n">
+    <row spans="1:1" r="2">
+      <c t="n" r="A2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="n">
+    <row spans="1:1" r="3">
+      <c t="n" r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="n">
+    <row spans="1:1" r="4">
+      <c t="n" r="A4">
         <v>4</v>
       </c>
     </row>
@@ -1934,38 +1934,38 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
+    <col min="1" width="9.10" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="n">
+    <row spans="1:1" r="1">
+      <c t="n" r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="n">
+    <row spans="1:1" r="2">
+      <c t="n" r="A2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="n">
+    <row spans="1:1" r="3">
+      <c t="n" r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="n">
+    <row spans="1:1" r="4">
+      <c t="n" r="A4">
         <v>4</v>
       </c>
     </row>
@@ -1975,99 +1975,99 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
+    <col min="1" width="9.10" max="1"/>
+    <col min="2" width="9.10" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="n">
+    <row spans="1:2" r="1">
+      <c t="n" r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="n">
+      <c t="n" r="B1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="n">
+    <row spans="1:2" r="2">
+      <c t="n" r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="n">
+    <row spans="1:2" r="3">
+      <c t="n" r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="n">
+    <row spans="1:2" r="4">
+      <c t="n" r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c t="n" r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="n">
+    <row spans="1:2" r="5">
+      <c t="n" r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c t="n" r="B5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="n">
+    <row spans="1:2" r="6">
+      <c t="n" r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
+      <c t="n" r="B6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="n">
+    <row spans="1:2" r="7">
+      <c t="n" r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c t="n" r="B7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="n">
+    <row spans="1:2" r="8">
+      <c t="n" r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c t="n" r="B8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="n">
+    <row spans="1:2" r="9">
+      <c t="n" r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
+      <c t="n" r="B9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="n">
+    <row spans="1:2" r="10">
+      <c t="n" r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
+      <c t="n" r="B10">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed other mistaken changes
--HG--
branch : 1.8
extra : rebase_source : 5a3e15b1d7183ad9dedc5730a7b0c3c69ffb0fef
</commit_message>
<xml_diff>
--- a/openpyxl/sample/files/charts.xlsx
+++ b/openpyxl/sample/files/charts.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <s:bookViews>
     <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet name="Numbers" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Negative" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Letters" sheetId="3" r:id="rId3"/>
-    <s:sheet name="Dates" sheetId="4" r:id="rId4"/>
-    <s:sheet name="Pie" sheetId="5" r:id="rId5"/>
-    <s:sheet name="Line" sheetId="6" r:id="rId6"/>
-    <s:sheet name="Scatter" sheetId="7" r:id="rId7"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Numbers" sheetId="1" r:id="rId1"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Negative" sheetId="2" r:id="rId2"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Letters" sheetId="3" r:id="rId3"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dates" sheetId="4" r:id="rId4"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pie" sheetId="5" r:id="rId5"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Line" sheetId="6" r:id="rId6"/>
+    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Scatter" sheetId="7" r:id="rId7"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -1066,7 +1066,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1076,12 +1076,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1091,7 +1091,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1101,12 +1101,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1116,7 +1116,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1126,12 +1126,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1141,7 +1141,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1151,12 +1151,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1166,7 +1166,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1176,12 +1176,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1191,7 +1191,7 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1201,12 +1201,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1216,7 +1216,7 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:absoluteAnchor>
     <xdr:pos x="95250" y="3810000"/>
     <xdr:ext cx="7620000" cy="3810000"/>
@@ -1226,12 +1226,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" x="0" y="0"/>
+        <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" cx="0" cy="0"/>
       </xdr:xfrm>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1245,10 +1245,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1404,7 +1404,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1413,13 +1413,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1429,7 +1429,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1438,7 +1438,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1447,7 +1447,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1457,12 +1457,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1493,7 +1493,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1512,7 +1512,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1524,68 +1524,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.10" max="1"/>
+    <col min="1" max="1" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:1" r="1">
-      <c t="n" r="A1">
+    <row r="1" spans="1:1">
+      <c r="A1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:1" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:1">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:1" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:1">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:1" r="4">
-      <c t="n" r="A4">
+    <row r="4" spans="1:1">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:1" r="5">
-      <c t="n" r="A5">
+    <row r="5" spans="1:1">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
     </row>
-    <row spans="1:1" r="6">
-      <c t="n" r="A6">
+    <row r="6" spans="1:1">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
     </row>
-    <row spans="1:1" r="7">
-      <c t="n" r="A7">
+    <row r="7" spans="1:1">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
     </row>
-    <row spans="1:1" r="8">
-      <c t="n" r="A8">
+    <row r="8" spans="1:1">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:1" r="9">
-      <c t="n" r="A9">
+    <row r="9" spans="1:1">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
     </row>
-    <row spans="1:1" r="10">
-      <c t="n" r="A10">
+    <row r="10" spans="1:1">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1595,68 +1595,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.10" max="1"/>
+    <col min="1" max="1" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:1" r="1">
-      <c t="n" r="A1">
+    <row r="1" spans="1:1">
+      <c r="A1" t="n">
         <v>-5</v>
       </c>
     </row>
-    <row spans="1:1" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:1">
+      <c r="A2" t="n">
         <v>-4</v>
       </c>
     </row>
-    <row spans="1:1" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:1">
+      <c r="A3" t="n">
         <v>-3</v>
       </c>
     </row>
-    <row spans="1:1" r="4">
-      <c t="n" r="A4">
+    <row r="4" spans="1:1">
+      <c r="A4" t="n">
         <v>-2</v>
       </c>
     </row>
-    <row spans="1:1" r="5">
-      <c t="n" r="A5">
+    <row r="5" spans="1:1">
+      <c r="A5" t="n">
         <v>-1</v>
       </c>
     </row>
-    <row spans="1:1" r="6">
-      <c t="n" r="A6">
+    <row r="6" spans="1:1">
+      <c r="A6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:1" r="7">
-      <c t="n" r="A7">
+    <row r="7" spans="1:1">
+      <c r="A7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:1" r="8">
-      <c t="n" r="A8">
+    <row r="8" spans="1:1">
+      <c r="A8" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:1" r="9">
-      <c t="n" r="A9">
+    <row r="9" spans="1:1">
+      <c r="A9" t="n">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:1" r="10">
-      <c t="n" r="A10">
+    <row r="10" spans="1:1">
+      <c r="A10" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1666,130 +1666,130 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.10" max="1"/>
-    <col min="3" width="9.10" max="3"/>
-    <col min="2" width="9.10" max="2"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="3" max="3" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c t="n" r="B1">
+      <c r="B1" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="C1">
+      <c r="C1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c t="n" r="C2">
+      <c r="C2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="s" r="A3">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:3" r="4">
-      <c t="s" r="A4">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c t="n" r="B4">
+      <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c t="n" r="C4">
+      <c r="C4" t="n">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:3" r="5">
-      <c t="s" r="A5">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c t="n" r="B5">
+      <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c t="n" r="C5">
+      <c r="C5" t="n">
         <v>4</v>
       </c>
     </row>
-    <row spans="1:3" r="6">
-      <c t="s" r="A6">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c t="n" r="B6">
+      <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c t="n" r="C6">
+      <c r="C6" t="n">
         <v>5</v>
       </c>
     </row>
-    <row spans="1:3" r="7">
-      <c t="s" r="A7">
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c t="n" r="B7">
+      <c r="B7" t="n">
         <v>6</v>
       </c>
-      <c t="n" r="C7">
+      <c r="C7" t="n">
         <v>6</v>
       </c>
     </row>
-    <row spans="1:3" r="8">
-      <c t="s" r="A8">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c t="n" r="B8">
+      <c r="B8" t="n">
         <v>7</v>
       </c>
-      <c t="n" r="C8">
+      <c r="C8" t="n">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:3" r="9">
-      <c t="s" r="A9">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c t="n" r="B9">
+      <c r="B9" t="n">
         <v>8</v>
       </c>
-      <c t="n" r="C9">
+      <c r="C9" t="n">
         <v>8</v>
       </c>
     </row>
-    <row spans="1:3" r="10">
-      <c t="s" r="A10">
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c t="n" r="B10">
+      <c r="B10" t="n">
         <v>9</v>
       </c>
-      <c t="n" r="C10">
+      <c r="C10" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1799,91 +1799,91 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.10" max="1"/>
-    <col min="2" width="9.10" max="2"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:2" r="1">
-      <c t="n" r="A1" s="1">
+    <row r="1" spans="1:2">
+      <c s="1" r="A1" t="n">
         <v>41275.0</v>
       </c>
-      <c t="n" r="B1">
+      <c r="B1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:2" r="2">
-      <c t="n" r="A2" s="1">
+    <row r="2" spans="1:2">
+      <c s="1" r="A2" t="n">
         <v>41306.0</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:2" r="3">
-      <c t="n" r="A3" s="1">
+    <row r="3" spans="1:2">
+      <c s="1" r="A3" t="n">
         <v>41334.0</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3" t="n">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:2" r="4">
-      <c t="n" r="A4" s="1">
+    <row r="4" spans="1:2">
+      <c s="1" r="A4" t="n">
         <v>41365.0</v>
       </c>
-      <c t="n" r="B4">
+      <c r="B4" t="n">
         <v>4</v>
       </c>
     </row>
-    <row spans="1:2" r="5">
-      <c t="n" r="A5" s="1">
+    <row r="5" spans="1:2">
+      <c s="1" r="A5" t="n">
         <v>41395.0</v>
       </c>
-      <c t="n" r="B5">
+      <c r="B5" t="n">
         <v>5</v>
       </c>
     </row>
-    <row spans="1:2" r="6">
-      <c t="n" r="A6" s="1">
+    <row r="6" spans="1:2">
+      <c s="1" r="A6" t="n">
         <v>41426.0</v>
       </c>
-      <c t="n" r="B6">
+      <c r="B6" t="n">
         <v>6</v>
       </c>
     </row>
-    <row spans="1:2" r="7">
-      <c t="n" r="A7" s="1">
+    <row r="7" spans="1:2">
+      <c s="1" r="A7" t="n">
         <v>41456.0</v>
       </c>
-      <c t="n" r="B7">
+      <c r="B7" t="n">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:2" r="8">
-      <c t="n" r="A8" s="1">
+    <row r="8" spans="1:2">
+      <c s="1" r="A8" t="n">
         <v>41487.0</v>
       </c>
-      <c t="n" r="B8">
+      <c r="B8" t="n">
         <v>8</v>
       </c>
     </row>
-    <row spans="1:2" r="9">
-      <c t="n" r="A9" s="1">
+    <row r="9" spans="1:2">
+      <c s="1" r="A9" t="n">
         <v>41518.0</v>
       </c>
-      <c t="n" r="B9">
+      <c r="B9" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1893,38 +1893,38 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.10" max="1"/>
+    <col min="1" max="1" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:1" r="1">
-      <c t="n" r="A1">
+    <row r="1" spans="1:1">
+      <c r="A1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:1" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:1">
+      <c r="A2" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:1" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:1">
+      <c r="A3" t="n">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:1" r="4">
-      <c t="n" r="A4">
+    <row r="4" spans="1:1">
+      <c r="A4" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1934,38 +1934,38 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.10" max="1"/>
+    <col min="1" max="1" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:1" r="1">
-      <c t="n" r="A1">
+    <row r="1" spans="1:1">
+      <c r="A1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:1" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:1">
+      <c r="A2" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:1" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:1">
+      <c r="A3" t="n">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:1" r="4">
-      <c t="n" r="A4">
+    <row r="4" spans="1:1">
+      <c r="A4" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1975,99 +1975,99 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.10" max="1"/>
-    <col min="2" width="9.10" max="2"/>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:2" r="1">
-      <c t="n" r="A1">
+    <row r="1" spans="1:2">
+      <c r="A1" t="n">
         <v>0</v>
       </c>
-      <c t="n" r="B1">
+      <c r="B1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:2" r="2">
-      <c t="n" r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row spans="1:2" r="3">
-      <c t="n" r="A3">
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row spans="1:2" r="4">
-      <c t="n" r="A4">
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c t="n" r="B4">
+      <c r="B4" t="n">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:2" r="5">
-      <c t="n" r="A5">
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c t="n" r="B5">
+      <c r="B5" t="n">
         <v>4</v>
       </c>
     </row>
-    <row spans="1:2" r="6">
-      <c t="n" r="A6">
+    <row r="6" spans="1:2">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c t="n" r="B6">
+      <c r="B6" t="n">
         <v>5</v>
       </c>
     </row>
-    <row spans="1:2" r="7">
-      <c t="n" r="A7">
+    <row r="7" spans="1:2">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c t="n" r="B7">
+      <c r="B7" t="n">
         <v>6</v>
       </c>
     </row>
-    <row spans="1:2" r="8">
-      <c t="n" r="A8">
+    <row r="8" spans="1:2">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c t="n" r="B8">
+      <c r="B8" t="n">
         <v>7</v>
       </c>
     </row>
-    <row spans="1:2" r="9">
-      <c t="n" r="A9">
+    <row r="9" spans="1:2">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c t="n" r="B9">
+      <c r="B9" t="n">
         <v>8</v>
       </c>
     </row>
-    <row spans="1:2" r="10">
-      <c t="n" r="A10">
+    <row r="10" spans="1:2">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c t="n" r="B10">
+      <c r="B10" t="n">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Restrict Series and References to cells with values. Updated sample file which no longer causes problems in Windows.
--HG--
branch : 1.8
</commit_message>
<xml_diff>
--- a/openpyxl/sample/files/charts.xlsx
+++ b/openpyxl/sample/files/charts.xlsx
@@ -342,10 +342,9 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Letters'!$A$1:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
@@ -377,8 +376,8 @@
                 <c:pt idx="9">
                   <c:v>J</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -424,10 +423,9 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Letters'!$A$1:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>A</c:v>
@@ -459,8 +457,8 @@
                 <c:pt idx="9">
                   <c:v>J</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -573,10 +571,10 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Dates'!$A$1:$A$10</c:f>
+              <c:f>'Dates'!$A$1:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>d-mmm</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>41275</c:v>
                 </c:pt>
@@ -603,19 +601,16 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>41518</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>None</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Dates'!$B$1:$B$10</c:f>
+              <c:f>'Dates'!$B$1:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -642,9 +637,6 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>None</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,10 +712,10 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Pie'!$A$1:$A$10</c:f>
+              <c:f>'Pie'!$A$1:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -735,34 +727,16 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>None</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pie'!$A$1:$A$10</c:f>
+              <c:f>'Pie'!$A$1:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -774,24 +748,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>None</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -836,10 +792,10 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Line'!$A$1:$A$5</c:f>
+              <c:f>'Line'!$A$1:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -851,9 +807,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>None</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,10 +882,10 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>'Scatter'!$B$1:$B$11</c:f>
+              <c:f>'Scatter'!$B$1:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -962,19 +915,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>None</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Scatter'!$A$1:$A$11</c:f>
+              <c:f>'Scatter'!$A$1:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1004,9 +954,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>None</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1679,8 +1626,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
     <col min="3" max="3" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1799,6 +1746,182 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c s="1" r="A1" t="n">
+        <v>41275.0</v>
+      </c>
+      <c r="B1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c s="1" r="A2" t="n">
+        <v>41306.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c s="1" r="A3" t="n">
+        <v>41334.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c s="1" r="A4" t="n">
+        <v>41365.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c s="1" r="A5" t="n">
+        <v>41395.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c s="1" r="A6" t="n">
+        <v>41426.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c s="1" r="A7" t="n">
+        <v>41456.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c s="1" r="A8" t="n">
+        <v>41487.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c s="1" r="A9" t="n">
+        <v>41518.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
@@ -1816,182 +1939,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c s="1" r="A1" t="n">
-        <v>41275.0</v>
-      </c>
-      <c r="B1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c s="1" r="A2" t="n">
-        <v>41306.0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c s="1" r="A3" t="n">
-        <v>41334.0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c s="1" r="A4" t="n">
-        <v>41365.0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c s="1" r="A5" t="n">
-        <v>41395.0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c s="1" r="A6" t="n">
-        <v>41426.0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c s="1" r="A7" t="n">
-        <v>41456.0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c s="1" r="A8" t="n">
-        <v>41487.0</v>
-      </c>
-      <c r="B8" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c s="1" r="A9" t="n">
-        <v>41518.0</v>
-      </c>
-      <c r="B9" t="n">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
-  </sheetPr>
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
-  </sheetPr>
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
-  </sheetPr>
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
       <c r="A1" t="n">
         <v>0</v>
       </c>

</xml_diff>